<commit_message>
Updated read-me, moved maersk notebook
Explaining maersk in read-me. Moved maersk notebook to notebook file.
</commit_message>
<xml_diff>
--- a/administration/Uren log.xlsx
+++ b/administration/Uren log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\shipping-data\administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819677CA-B294-491A-B1C8-7FE121A59006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6D7233-2D59-4968-8B5A-E9E7AE07B43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ewout" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>Wanneer</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Working towars automatization</t>
+  </si>
+  <si>
+    <t>Finishing Maersk scraper</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC13614-0EFB-42A2-B55B-3B7A8DE84ACE}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,8 +493,8 @@
         <v>0.5</v>
       </c>
       <c r="E3">
-        <f>SUM(C2:C25)</f>
-        <v>35.5</v>
+        <f>SUM(C2:C30)</f>
+        <v>37.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -679,6 +682,17 @@
       </c>
       <c r="C20">
         <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44883</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maersk updated dataframe to new format
Performed a lot of work of reworking the dataframe to the new format
</commit_message>
<xml_diff>
--- a/administration/Uren log.xlsx
+++ b/administration/Uren log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\shipping-data\administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E410190-3B5C-4F20-A59C-90947DC03871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC1B0C0-B535-4B23-B3F2-688CE12CC2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ewout" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Wanneer</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Combining Maersk, file structure, bugfixing</t>
+  </si>
+  <si>
+    <t>Gewerkt</t>
+  </si>
+  <si>
+    <t>Gedeclareerd</t>
+  </si>
+  <si>
+    <t>Meeting data formatting MSC Maersk Routescanner</t>
+  </si>
+  <si>
+    <t>Combining dataframes in python</t>
   </si>
 </sst>
 </file>
@@ -466,10 +478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC13614-0EFB-42A2-B55B-3B7A8DE84ACE}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +490,7 @@
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -492,7 +504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -506,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -521,10 +533,13 @@
       </c>
       <c r="E3">
         <f>SUM(C2:C30)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -538,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -552,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -566,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -580,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -594,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -608,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -622,7 +637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -636,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -650,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -664,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -678,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -692,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -706,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -720,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -734,11 +749,14 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <f>SUM(C2:C18)</f>
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <f>SUM(C2:C21)</f>
+        <v>37.5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -752,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -766,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -780,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -791,7 +809,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -802,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -813,7 +831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -822,6 +840,28 @@
       </c>
       <c r="C25">
         <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44943</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44965</v>
+      </c>
+      <c r="C27">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maersk put changes from notebook to .py
The changes that were made to the notebook were not put in the .py. Now that is fixed
</commit_message>
<xml_diff>
--- a/administration/Uren log.xlsx
+++ b/administration/Uren log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\shipping-data\administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC1B0C0-B535-4B23-B3F2-688CE12CC2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D586A2-27B6-4FE3-86CF-FE58EBD30C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Wanneer</t>
   </si>
@@ -478,7 +478,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC13614-0EFB-42A2-B55B-3B7A8DE84ACE}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -532,8 +532,8 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <f>SUM(C2:C30)</f>
-        <v>47.5</v>
+        <f>SUM(C2:C35)</f>
+        <v>50.5</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -862,6 +862,17 @@
       </c>
       <c r="C27">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44973</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>